<commit_message>
Add condition formats to the template Fixed default translation
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github\arb_sheet\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\free-mind\games\admin\assets\l10n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC493AD-8DAB-4620-8E20-A8234C0E0AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F20AB6-7B54-4111-8AC5-4B22B75E5F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15564" yWindow="2724" windowWidth="15108" windowHeight="12888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4464" yWindow="1776" windowWidth="15108" windowHeight="12888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
+    <sheet name="Note" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t>category</t>
   </si>
@@ -43,12 +44,6 @@
     <t>welcome</t>
   </si>
   <si>
-    <t>Hi, {gender} {name}</t>
-  </si>
-  <si>
-    <t>Xin chào, {gender} {name}</t>
-  </si>
-  <si>
     <t>support</t>
   </si>
   <si>
@@ -73,19 +68,157 @@
     <t>Chiến dịch</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>campaigns</t>
-  </si>
-  <si>
-    <t>The app title</t>
-  </si>
-  <si>
     <t>Ez-Connect</t>
   </si>
   <si>
     <t>Welcome</t>
+  </si>
+  <si>
+    <t>FREEMIND</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>The company title</t>
+  </si>
+  <si>
+    <t>Hi, {name}</t>
+  </si>
+  <si>
+    <t>Xin chào, {name}</t>
+  </si>
+  <si>
+    <t>analytics</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>game</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Subcription Setting</t>
+  </si>
+  <si>
+    <t>subscriptionSetting</t>
+  </si>
+  <si>
+    <t>Payment History</t>
+  </si>
+  <si>
+    <t>paymentHistory</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Log Out</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>campaignList</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>To review</t>
+  </si>
+  <si>
+    <t>To translated</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Họ</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Quốc gia</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Tài khoản</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Lịch sử giao dịch</t>
+  </si>
+  <si>
+    <t>Nâng cấp</t>
+  </si>
+  <si>
+    <t>Thống kê</t>
+  </si>
+  <si>
+    <t>Duplicate text</t>
+  </si>
+  <si>
+    <t>Condition format: blank value</t>
+  </si>
+  <si>
+    <t>Condition format: duplicate values</t>
   </si>
 </sst>
 </file>
@@ -228,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +539,24 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -569,8 +720,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -616,7 +770,69 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -630,8 +846,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0">
+  <autoFilter ref="A1:E18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="text"/>
@@ -640,6 +856,18 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="vi"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8FC3499-12BC-435E-BB6E-72634892E2D2}" name="Table2" displayName="Table2" ref="B2:D6" totalsRowShown="0">
+  <autoFilter ref="B2:D6" xr:uid="{C8FC3499-12BC-435E-BB6E-72634892E2D2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DA4621A8-96BC-436C-9FE8-B6EC06E2D61D}" name="Status"/>
+    <tableColumn id="2" xr3:uid="{C1CD239F-4F43-42AD-B4D1-106DCAB44A1B}" name="Color"/>
+    <tableColumn id="3" xr3:uid="{DA2BF46A-9EAE-4EE3-B6FE-4449245638CF}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -940,17 +1168,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
   </cols>
@@ -977,16 +1205,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -997,13 +1225,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1011,10 +1239,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1022,31 +1250,270 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
         <v>14</v>
       </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:Z12 E16:Z1048576 F13:Z15">
+    <cfRule type="containsBlanks" dxfId="1" priority="5">
+      <formula>LEN(TRIM(E1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB689139-3580-4870-A345-8D844F82E48B}">
+  <dimension ref="B1:D6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="0.8984375" customWidth="1"/>
+    <col min="2" max="2" width="12.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="7.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>